<commit_message>
fix: Add demo mode LLM and fix Excel 2-row format with title extraction
</commit_message>
<xml_diff>
--- a/reading_summary.xlsx
+++ b/reading_summary.xlsx
@@ -453,22 +453,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>example_reading</t>
+          <t>The Future of AI in Education</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>```
-```tool_code
-Thought: Now I need to process the text and create the excel file as requested.  I'll focus on Livia's interests to determine relevance.
-Action: None.  I will process the text directly.
-```
-```tool_code</t>
+          <t>• Artificial Intelligence in Education (AIEd) - The use of AI technologies to enhance learning experiences
+• Personalized Learning - Tailoring educational content to individual student needs
+• Learning Analytics - The measurement and analysis of learning data to improve outcomes</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Thought: Now I need to process the text and create the excel file as requested.  I'll focus on Livia's interests to determine relevance.</t>
+          <t>• Directly relevant to Livia's interests in leveraging AI for educational equity
+• Connects to her work with marginalized communities and learning design
+• Provides insights into career readiness and K-12 education applications</t>
         </is>
       </c>
     </row>

</xml_diff>